<commit_message>
Updated Steam test cases with validations
</commit_message>
<xml_diff>
--- a/src/test/test-data/STeAMTestData.xlsx
+++ b/src/test/test-data/STeAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
   <si>
     <t>STATUS</t>
   </si>
@@ -94,9 +94,6 @@
     <t>OPQA-CCC</t>
   </si>
   <si>
-    <t>status=200||rc=OK||USER.USER_ID=(OPQA-AAA_user.userID)</t>
-  </si>
-  <si>
     <t>UpdateUserDetails</t>
   </si>
   <si>
@@ -133,9 +130,6 @@
     <t>USERNAME=Neon_JDRUser4@1p.com||PASSWORD=1234qwer$$!</t>
   </si>
   <si>
-    <t>status=200||rc=OK||User.isActive=YES||User.userID=(OPQA-AAA_user.userID)||User.truId=(OPQA-AAA_user.truID)</t>
-  </si>
-  <si>
     <t>OPQA-FFF</t>
   </si>
   <si>
@@ -187,17 +181,19 @@
     <t>status=200||rc=OK||Results.USER_ID=(OPQA-AAA_user.userID)||Results.TRUID=(OPQA-AAA_user.truID)||Results.TOTAL_ROWS=1</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>status=200||rc=OK||USER.USER_ID=(OPQA-AAA_user.userID)||UserInfo.USER_INFO_FIRST_NAME=JANARDHANUpadateF||UserInfo.USER_INFO_MIDDLE_NAME=REDDYUpdatedM||UserInfo.USER_INFO_LAST_NAME=UpdatedL</t>
+  </si>
+  <si>
+    <t>UserInfo.USER_INFO_FIRST_NAME||UserInfo.USER_INFO_MIDDLE_NAME||UserInfo.USER_INFO_LAST_NAME</t>
+  </si>
+  <si>
+    <t>status=200||rc=OK||User.isActive=YES||User.userID=(OPQA-AAA_user.userID)||User.truId=(OPQA-AAA_user.truID)||UserInfo.USER_INFO_FIRST_NAME=(OPQA-CCC_UserInfo.USER_INFO_FIRST_NAME)||UserInfo.USER_INFO_MIDDLE_NAME=(OPQA-CCC_UserInfo.USER_INFO_MIDDLE_NAME)||UserInfo.USER_INFO_LAST_NAME=(OPQA-CCC_UserInfo.USER_INFO_LAST_NAME)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -276,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -302,6 +298,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,19 +603,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="49.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="52.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="40.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="5" width="80.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="53.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="52.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="80.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="54.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="26.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -653,7 +652,7 @@
       <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -688,11 +687,8 @@
       <c r="K2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="M2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="45">
@@ -726,16 +722,13 @@
         <v>21</v>
       </c>
       <c r="L3"/>
-      <c r="M3" t="s">
-        <v>58</v>
-      </c>
     </row>
-    <row r="4" spans="1:13" ht="31.5">
+    <row r="4" spans="1:13" ht="75">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>17</v>
@@ -749,28 +742,27 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4"/>
-      <c r="M4" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="31.5">
       <c r="A5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>17</v>
@@ -784,28 +776,25 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L5"/>
-      <c r="M5" t="s">
-        <v>58</v>
-      </c>
     </row>
-    <row r="6" spans="1:13" ht="45">
+    <row r="6" spans="1:13" ht="135">
       <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>17</v>
@@ -819,28 +808,25 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
         <v>37</v>
       </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
       <c r="J6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="L6"/>
-      <c r="M6" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="7" spans="1:13" ht="31.5">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>17</v>
@@ -854,28 +840,25 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L7"/>
-      <c r="M7" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="8" spans="1:13" ht="31.5">
       <c r="A8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>17</v>
@@ -889,28 +872,25 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L8"/>
-      <c r="M8" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="9" spans="1:13" ht="45">
       <c r="A9" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>17</v>
@@ -924,26 +904,23 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I9"/>
       <c r="J9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L9"/>
-      <c r="M9" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="10" spans="1:13" ht="31.5">
       <c r="A10" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>17</v>
@@ -957,7 +934,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I10"/>
       <c r="J10" s="6" t="s">
@@ -967,9 +944,6 @@
         <v>23</v>
       </c>
       <c r="L10"/>
-      <c r="M10" t="s">
-        <v>58</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed failed steam test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/STeAMTestData.xlsx
+++ b/src/test/test-data/STeAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
   <si>
     <t>STATUS</t>
   </si>
@@ -106,15 +106,9 @@
     <t>OPQA-DDD</t>
   </si>
   <si>
-    <t>Verify that based on truid, user status can be updated using STeAM API</t>
-  </si>
-  <si>
     <t>ISACTIVE=YES</t>
   </si>
   <si>
-    <t>status=200||rc=OK||TRANSACTION.MESSAGE=1 Rows Updated||TRANSACTION.STATUS=PASS</t>
-  </si>
-  <si>
     <t>UpdateUserStatus</t>
   </si>
   <si>
@@ -187,7 +181,16 @@
     <t>UserInfo.USER_INFO_FIRST_NAME||UserInfo.USER_INFO_MIDDLE_NAME||UserInfo.USER_INFO_LAST_NAME</t>
   </si>
   <si>
-    <t>status=200||rc=OK||User.isActive=YES||User.userID=(OPQA-AAA_user.userID)||User.truId=(OPQA-AAA_user.truID)||UserInfo.USER_INFO_FIRST_NAME=(OPQA-CCC_UserInfo.USER_INFO_FIRST_NAME)||UserInfo.USER_INFO_MIDDLE_NAME=(OPQA-CCC_UserInfo.USER_INFO_MIDDLE_NAME)||UserInfo.USER_INFO_LAST_NAME=(OPQA-CCC_UserInfo.USER_INFO_LAST_NAME)</t>
+    <t>USER_NAME=Neon_JDRUser4@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=JANARDHAN4||USER_LAST_NAME=E4||USER_MIDDLE_NAME=REDDY4||USER_TRUID=c32994ec-6dcd-4884-ab42-682bbc0f9e8b</t>
+  </si>
+  <si>
+    <t>Verify that based on truid, user status can't be updated and check the error status using STeAM API</t>
+  </si>
+  <si>
+    <t>status=200||rc=55003||fn[1].error=Action UPDATE_NEON_USER_STATUS is not supported</t>
+  </si>
+  <si>
+    <t>status=200||rc=OK||User.userID=(OPQA-AAA_user.userID)||User.truId=(OPQA-AAA_user.truID)||UserInfo.USER_INFO_FIRST_NAME=(OPQA-CCC_UserInfo.USER_INFO_FIRST_NAME)||UserInfo.USER_INFO_MIDDLE_NAME=(OPQA-CCC_UserInfo.USER_INFO_MIDDLE_NAME)||UserInfo.USER_INFO_LAST_NAME=(OPQA-CCC_UserInfo.USER_INFO_LAST_NAME)</t>
   </si>
 </sst>
 </file>
@@ -659,7 +662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="45">
+    <row r="2" spans="1:13" ht="60">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -681,7 +684,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
@@ -751,10 +754,10 @@
         <v>12</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="31.5">
@@ -762,7 +765,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>17</v>
@@ -776,25 +779,25 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="L5"/>
     </row>
     <row r="6" spans="1:13" ht="135">
       <c r="A6" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>17</v>
@@ -808,25 +811,25 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L6"/>
     </row>
     <row r="7" spans="1:13" ht="31.5">
       <c r="A7" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>17</v>
@@ -840,25 +843,25 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" t="s">
         <v>39</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:13" ht="31.5">
       <c r="A8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>17</v>
@@ -872,25 +875,25 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L8"/>
     </row>
     <row r="9" spans="1:13" ht="45">
       <c r="A9" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>17</v>
@@ -904,23 +907,23 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I9"/>
       <c r="J9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L9"/>
     </row>
     <row r="10" spans="1:13" ht="31.5">
       <c r="A10" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>17</v>
@@ -934,7 +937,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I10"/>
       <c r="J10" s="6" t="s">

</xml_diff>

<commit_message>
Added new test cases for steam.
</commit_message>
<xml_diff>
--- a/src/test/test-data/STeAMTestData.xlsx
+++ b/src/test/test-data/STeAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
   <si>
     <t>STATUS</t>
   </si>
@@ -106,15 +106,9 @@
     <t>USERNAME=Neon_JDRUser4@1p.com||PASSWORD=1234qwer$$!</t>
   </si>
   <si>
-    <t>UNP_Username=Neon_JDRUser4@1p.com</t>
-  </si>
-  <si>
     <t>UpdateEmail</t>
   </si>
   <si>
-    <t>Verify that based on user ID, user email can be updated using STeAM API</t>
-  </si>
-  <si>
     <t>Verify that based on user's email, search results can be returned using STeAM API</t>
   </si>
   <si>
@@ -181,9 +175,6 @@
     <t>status=200||rc=OK||USER.USER_ID=(OPQA-1410_user.userID)||UserInfo.USER_INFO_FIRST_NAME=JANARDHANUpadateF||UserInfo.USER_INFO_MIDDLE_NAME=REDDYUpdatedM||UserInfo.USER_INFO_LAST_NAME=UpdatedL</t>
   </si>
   <si>
-    <t>status=200||rc=OK||user.userID=(OPQA-1410_user.userID)</t>
-  </si>
-  <si>
     <t>status=200||rc=OK||USER.UserId=(OPQA-1410_user.userID)</t>
   </si>
   <si>
@@ -191,6 +182,36 @@
   </si>
   <si>
     <t>status=200||rc=OK||User.userID=(OPQA-1410_user.userID)||User.truId=(OPQA-1410_user.truID)||UserInfo.USER_INFO_FIRST_NAME=(OPQA-1412_UserInfo.USER_INFO_FIRST_NAME)||UserInfo.USER_INFO_MIDDLE_NAME=(OPQA-1412_UserInfo.USER_INFO_MIDDLE_NAME)||UserInfo.USER_INFO_LAST_NAME=(OPQA-1412_UserInfo.USER_INFO_LAST_NAME)</t>
+  </si>
+  <si>
+    <t>Verify that based on user ID, user email and password can be updated using STeAM API</t>
+  </si>
+  <si>
+    <t>UNP_Username=Neon_JDRUser4@1p.com||UNP_Password=1234qwer$#</t>
+  </si>
+  <si>
+    <t>status=200||rc=OK||user.userID=(OPQA-1410_user.userID)||USER_UsernamePasswordCredential.userName=Neon_JDRUser4@1p.com</t>
+  </si>
+  <si>
+    <t>USER_UsernamePasswordCredential.userName</t>
+  </si>
+  <si>
+    <t>Verify that deleted user details can't be deleted again and check the error status using STeAM API</t>
+  </si>
+  <si>
+    <t>status=200||rc=30000||fn[1].error=UserId does not exist or User has been deleted</t>
+  </si>
+  <si>
+    <t>Verify that same password can't be updated for the user id and check the error status using STeAM API</t>
+  </si>
+  <si>
+    <t>status=200||rc=50181||fn[1].error=New password should not match current password</t>
+  </si>
+  <si>
+    <t>OPQA-1591</t>
+  </si>
+  <si>
+    <t>OPQA-1592</t>
   </si>
 </sst>
 </file>
@@ -598,15 +619,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M10"/>
+    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
+      <selection activeCell="M12" sqref="M2:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -664,7 +685,7 @@
     </row>
     <row r="2" spans="1:13" ht="60">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>14</v>
@@ -684,7 +705,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
@@ -696,10 +717,10 @@
     </row>
     <row r="3" spans="1:13" ht="45">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>16</v>
@@ -719,7 +740,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>20</v>
@@ -728,7 +749,7 @@
     </row>
     <row r="4" spans="1:13" ht="75">
       <c r="A4" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>23</v>
@@ -751,21 +772,21 @@
         <v>24</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="31.5">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>16</v>
@@ -785,16 +806,16 @@
         <v>25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L5"/>
     </row>
     <row r="6" spans="1:13" ht="135">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>27</v>
@@ -817,19 +838,19 @@
         <v>29</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:13" ht="31.5">
+    <row r="7" spans="1:13" ht="45">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>16</v>
@@ -843,25 +864,27 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="I7" t="s">
+        <v>57</v>
+      </c>
       <c r="J7" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7"/>
+        <v>58</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="31.5">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>16</v>
@@ -875,25 +898,25 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>48</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="1:13" ht="45">
+        <v>63</v>
+      </c>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" ht="31.5">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>16</v>
@@ -907,23 +930,25 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9"/>
+        <v>33</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="J9" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:13" ht="31.5">
+    <row r="10" spans="1:13" ht="45">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>16</v>
@@ -937,16 +962,74 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I10"/>
       <c r="J10" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="1:13" ht="31.5">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L10"/>
+      <c r="L11"/>
+    </row>
+    <row r="12" spans="1:13" ht="31.5">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12"/>
+      <c r="J12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated pending STeAM test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/STeAMTestData.xlsx
+++ b/src/test/test-data/STeAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
   <si>
     <t>STATUS</t>
   </si>
@@ -214,9 +214,6 @@
     <t>OPQA-1592</t>
   </si>
   <si>
-    <t>Verify that locked user can be unlocked using UnlockNeonUser STeAM API.</t>
-  </si>
-  <si>
     <t>UnlockNeonUser</t>
   </si>
   <si>
@@ -236,6 +233,30 @@
   </si>
   <si>
     <t>OPQA-1608</t>
+  </si>
+  <si>
+    <t>Verify that for the given STeAM UID, locked user can be unlocked using UnlockNeonUser STeAM API.</t>
+  </si>
+  <si>
+    <t>Verify that for the given email id, locked user can be unlocked using UnlockNeonUser STeAM API.</t>
+  </si>
+  <si>
+    <t>UnlockNeonUserBasedOnEmail</t>
+  </si>
+  <si>
+    <t>OPQA-1609</t>
+  </si>
+  <si>
+    <t>Verify that new user can't be created with duplicate TRUID and check the error status using STeAM API</t>
+  </si>
+  <si>
+    <t>USER_NAME=Neon_JDRUser5@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=JDR||USER_LAST_NAME=E5||USER_MIDDLE_NAME=REDDY5||USER_TRUID=c32994ec-6dcd-4884-ab42-682bbc0f9e8b</t>
+  </si>
+  <si>
+    <t>status=200||rc=90056||fn[1].error=TRUID cannot be duplicate</t>
+  </si>
+  <si>
+    <t>OPQA-1610</t>
   </si>
 </sst>
 </file>
@@ -643,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J7" workbookViewId="0">
-      <selection activeCell="M14" sqref="M2:M14"/>
+    <sheetView tabSelected="1" topLeftCell="J9" workbookViewId="0">
+      <selection activeCell="M16" sqref="M2:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -658,7 +679,7 @@
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="52.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="80.5703125" style="5" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="18.140625" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="54.85546875" customWidth="1" collapsed="1"/>
@@ -771,12 +792,12 @@
       </c>
       <c r="L3"/>
     </row>
-    <row r="4" spans="1:13" ht="75">
+    <row r="4" spans="1:13" ht="60">
       <c r="A4" s="6" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>16</v>
@@ -790,27 +811,25 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="31.5">
-      <c r="A5" t="s">
-        <v>46</v>
+        <v>79</v>
+      </c>
+      <c r="L4"/>
+    </row>
+    <row r="5" spans="1:13" ht="75">
+      <c r="A5" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>16</v>
@@ -824,25 +843,27 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>42</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5"/>
-    </row>
-    <row r="6" spans="1:13" ht="135">
+        <v>52</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="31.5">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>16</v>
@@ -856,25 +877,25 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>42</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:13" ht="45">
+    <row r="7" spans="1:13" ht="135">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>16</v>
@@ -888,27 +909,25 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" t="s">
-        <v>57</v>
+        <v>28</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>42</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="31.5">
+        <v>55</v>
+      </c>
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="1:13" ht="45">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>16</v>
@@ -927,20 +946,22 @@
       <c r="I8" t="s">
         <v>57</v>
       </c>
-      <c r="J8" t="s">
-        <v>48</v>
+      <c r="J8" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="L8" s="11"/>
+        <v>58</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="31.5">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>16</v>
@@ -954,25 +975,25 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" t="s">
+        <v>48</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="1:13" ht="45">
+        <v>63</v>
+      </c>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" ht="31.5">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>16</v>
@@ -986,23 +1007,25 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10"/>
+        <v>33</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="J10" s="6" t="s">
         <v>42</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L10"/>
     </row>
-    <row r="11" spans="1:13" ht="47.25">
+    <row r="11" spans="1:13" ht="45">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>16</v>
@@ -1016,25 +1039,23 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" t="s">
-        <v>70</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I11"/>
       <c r="J11" s="6" t="s">
         <v>42</v>
       </c>
       <c r="K11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11"/>
+    </row>
+    <row r="12" spans="1:13" ht="47.25">
+      <c r="A12" t="s">
         <v>71</v>
       </c>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:13" ht="31.5">
-      <c r="A12" t="s">
-        <v>73</v>
-      </c>
       <c r="B12" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>16</v>
@@ -1048,21 +1069,25 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12"/>
-      <c r="J12" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="K12" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L12"/>
     </row>
     <row r="13" spans="1:13" ht="31.5">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>16</v>
@@ -1076,44 +1101,100 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="I13"/>
-      <c r="J13" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="J13" s="6"/>
       <c r="K13" s="4" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:13" ht="31.5">
       <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="1:13" ht="31.5">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15"/>
+    </row>
+    <row r="16" spans="1:13" ht="31.5">
+      <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="C16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I14"/>
-      <c r="J14" t="s">
+      <c r="I16"/>
+      <c r="J16" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L14"/>
+      <c r="L16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated new test cases for STeAM API.
</commit_message>
<xml_diff>
--- a/src/test/test-data/STeAMTestData.xlsx
+++ b/src/test/test-data/STeAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="86">
   <si>
     <t>STATUS</t>
   </si>
@@ -73,9 +73,6 @@
     <t>user.userID||user.truID</t>
   </si>
   <si>
-    <t>USER_NAME=Neon_JDRUser4@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=JANARDHAN4||USER_LAST_NAME=E4||USER_MIDDLE_NAME=REDDY4</t>
-  </si>
-  <si>
     <t>status=200||rc=30047||fn[1].error=Username already exists in database</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Verify that based on user id, user details can be updated using STeAM API</t>
   </si>
   <si>
-    <t>USER_FIRST_NAME=JANARDHANUpadateF||USER_LAST_NAME=UpdatedL||USER_MIDDLE_NAME=REDDYUpdatedM</t>
-  </si>
-  <si>
     <t>ISACTIVE=YES</t>
   </si>
   <si>
@@ -103,18 +97,12 @@
     <t>GetLoginUNP</t>
   </si>
   <si>
-    <t>USERNAME=Neon_JDRUser4@1p.com||PASSWORD=1234qwer$$!</t>
-  </si>
-  <si>
     <t>UpdateEmail</t>
   </si>
   <si>
     <t>Verify that based on user's email, search results can be returned using STeAM API</t>
   </si>
   <si>
-    <t>EMAIL_ID=Neon_JDRUser4@1p.com</t>
-  </si>
-  <si>
     <t>SearchUserEmail</t>
   </si>
   <si>
@@ -169,9 +157,6 @@
     <t>OPQA-1418</t>
   </si>
   <si>
-    <t>status=200||rc=OK||USER.USER_ID=(OPQA-1410_user.userID)||UserInfo.USER_INFO_FIRST_NAME=JANARDHANUpadateF||UserInfo.USER_INFO_MIDDLE_NAME=REDDYUpdatedM||UserInfo.USER_INFO_LAST_NAME=UpdatedL</t>
-  </si>
-  <si>
     <t>status=200||rc=OK||USER.UserId=(OPQA-1410_user.userID)</t>
   </si>
   <si>
@@ -184,12 +169,6 @@
     <t>Verify that based on user ID, user email and password can be updated using STeAM API</t>
   </si>
   <si>
-    <t>UNP_Username=Neon_JDRUser4@1p.com||UNP_Password=1234qwer$#</t>
-  </si>
-  <si>
-    <t>status=200||rc=OK||user.userID=(OPQA-1410_user.userID)||USER_UsernamePasswordCredential.userName=Neon_JDRUser4@1p.com</t>
-  </si>
-  <si>
     <t>USER_UsernamePasswordCredential.userName</t>
   </si>
   <si>
@@ -220,9 +199,6 @@
     <t>Verify that with incorrect user name or password, user not able to login and check the error message using STeAM API.</t>
   </si>
   <si>
-    <t>USERNAME=Neon_JDRUser4@1p.com||PASSWORD=1234qwer$$!#</t>
-  </si>
-  <si>
     <t>status=200||rc=40012||fn[1].error=Login failed</t>
   </si>
   <si>
@@ -253,10 +229,49 @@
     <t>OPQA-1610</t>
   </si>
   <si>
-    <t>USER_NAME=Neon_JDRUser4@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=JANARDHAN4||USER_LAST_NAME=E4||USER_MIDDLE_NAME=REDDY4||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3235123</t>
-  </si>
-  <si>
     <t>USER_NAME=Neon_JDRUser5@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=JDR||USER_LAST_NAME=E5||USER_MIDDLE_NAME=REDDY5||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3235123</t>
+  </si>
+  <si>
+    <t>USER_NAME=Project_NeonUser1@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=Project||USER_LAST_NAME=Neon1||USER_MIDDLE_NAME=TR||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3235123</t>
+  </si>
+  <si>
+    <t>Verify that new STeAM user account can be created without first name, last name using STeAM API</t>
+  </si>
+  <si>
+    <t>USER_NAME=Neon_JDRUser6@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3235124</t>
+  </si>
+  <si>
+    <t>OPQA-1418_1</t>
+  </si>
+  <si>
+    <t>userID=(OPQA-1410_user.userID)</t>
+  </si>
+  <si>
+    <t>USER_FIRST_NAME=ProjectF||USER_LAST_NAME=UpdatedL||USER_MIDDLE_NAME=NeonM</t>
+  </si>
+  <si>
+    <t>status=200||rc=OK||USER.USER_ID=(OPQA-1410_user.userID)||UserInfo.USER_INFO_FIRST_NAME=ProjectF||UserInfo.USER_INFO_MIDDLE_NAME=NeonM||UserInfo.USER_INFO_LAST_NAME=UpdatedL</t>
+  </si>
+  <si>
+    <t>USERNAME=Project_NeonUser1@1p.com||PASSWORD=1234qwer$$!</t>
+  </si>
+  <si>
+    <t>UNP_Username=Project_NeonUser2@1p.com||UNP_Password=1234qwer$#</t>
+  </si>
+  <si>
+    <t>EMAIL_ID=Project_NeonUser2@1p.com</t>
+  </si>
+  <si>
+    <t>USERNAME=Project_NeonUser2@1p.com||PASSWORD=1234qwer$$!#</t>
+  </si>
+  <si>
+    <t>status=200||rc=OK||user.userID=(OPQA-1410_user.userID)||USER_UsernamePasswordCredential.userName=Project_NeonUser2@1p.com</t>
+  </si>
+  <si>
+    <t>OPQA-2407</t>
+  </si>
+  <si>
+    <t>userID=(OPQA-2407_user.userID)</t>
   </si>
 </sst>
 </file>
@@ -664,15 +679,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="M2" sqref="M2:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -730,7 +745,7 @@
     </row>
     <row r="2" spans="1:13" ht="60">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>14</v>
@@ -750,22 +765,22 @@
         <v>15</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="45">
+    <row r="3" spans="1:13" ht="60">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>16</v>
@@ -782,22 +797,22 @@
         <v>15</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="L3"/>
     </row>
-    <row r="4" spans="1:13" ht="60">
+    <row r="4" spans="1:13" ht="45">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>16</v>
@@ -814,22 +829,22 @@
         <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="L4"/>
-    </row>
-    <row r="5" spans="1:13" ht="75">
+        <v>20</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="60">
       <c r="A5" s="6" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>16</v>
@@ -843,27 +858,25 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5"/>
+    </row>
+    <row r="6" spans="1:13" ht="60">
+      <c r="A6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="31.5">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>16</v>
@@ -877,25 +890,27 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="J6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="31.5">
+      <c r="A7" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6"/>
-    </row>
-    <row r="7" spans="1:13" ht="135">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
       <c r="B7" s="9" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>16</v>
@@ -909,25 +924,25 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:13" ht="45">
+    <row r="8" spans="1:13" ht="135">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>16</v>
@@ -941,27 +956,25 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="31.5">
+        <v>49</v>
+      </c>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="1:13" ht="45">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>16</v>
@@ -975,25 +988,27 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" t="s">
-        <v>47</v>
+        <v>80</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" s="11"/>
+        <v>83</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="31.5">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>16</v>
@@ -1007,25 +1022,25 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
+      </c>
+      <c r="I10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" t="s">
+        <v>43</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10"/>
-    </row>
-    <row r="11" spans="1:13" ht="45">
+        <v>55</v>
+      </c>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:13" ht="31.5">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>16</v>
@@ -1039,23 +1054,25 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11"/>
+        <v>29</v>
+      </c>
+      <c r="I11" t="s">
+        <v>81</v>
+      </c>
       <c r="J11" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:13" ht="47.25">
+    <row r="12" spans="1:13" ht="45">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>16</v>
@@ -1069,25 +1086,23 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" t="s">
-        <v>68</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="I12"/>
       <c r="J12" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:13" ht="31.5">
+    <row r="13" spans="1:13" ht="47.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>16</v>
@@ -1101,21 +1116,25 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13"/>
-      <c r="J13" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="K13" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:13" ht="31.5">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>16</v>
@@ -1129,21 +1148,21 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="I14"/>
       <c r="J14" s="6"/>
       <c r="K14" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="L14"/>
     </row>
     <row r="15" spans="1:13" ht="31.5">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>16</v>
@@ -1157,23 +1176,21 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="I15"/>
-      <c r="J15" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="J15" s="6"/>
       <c r="K15" s="4" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="L15"/>
     </row>
     <row r="16" spans="1:13" ht="31.5">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>16</v>
@@ -1184,17 +1201,83 @@
       <c r="E16" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I16"/>
-      <c r="J16" t="s">
-        <v>50</v>
-      </c>
       <c r="K16" s="4" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="L16"/>
+    </row>
+    <row r="17" spans="1:12" ht="31.5">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:12" ht="31.5">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed failed STeAM-Neon test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/STeAMTestData.xlsx
+++ b/src/test/test-data/STeAMTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="86">
   <si>
     <t>STATUS</t>
   </si>
@@ -681,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J8" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:M18"/>
     </sheetView>
   </sheetViews>
@@ -1151,7 +1151,9 @@
         <v>58</v>
       </c>
       <c r="I14"/>
-      <c r="J14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="K14" s="4" t="s">
         <v>59</v>
       </c>
@@ -1179,7 +1181,9 @@
         <v>66</v>
       </c>
       <c r="I15"/>
-      <c r="J15" s="6"/>
+      <c r="J15" t="s">
+        <v>43</v>
+      </c>
       <c r="K15" s="4" t="s">
         <v>59</v>
       </c>
@@ -1280,7 +1284,11 @@
       <c r="L18"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed steam failed test case. OPQA-1607
</commit_message>
<xml_diff>
--- a/src/test/test-data/STeAMTestData.xlsx
+++ b/src/test/test-data/STeAMTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UC196992\Git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
@@ -199,9 +204,6 @@
     <t>Verify that with incorrect user name or password, user not able to login and check the error message using STeAM API.</t>
   </si>
   <si>
-    <t>status=200||rc=40012||fn[1].error=Login failed</t>
-  </si>
-  <si>
     <t>OPQA-1607</t>
   </si>
   <si>
@@ -272,13 +274,16 @@
   </si>
   <si>
     <t>userID=(OPQA-2407_user.userID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status=200||rc=90063||fn[1].error=Login Failed.  9 more chances are remaining, after that your account will be locked. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,6 +396,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -437,7 +450,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,9 +482,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -503,6 +517,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -678,14 +693,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J8" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M18"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
@@ -702,7 +717,7 @@
     <col min="13" max="13" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -743,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60">
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
@@ -765,7 +780,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
@@ -774,8 +789,9 @@
       <c r="L2" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="60">
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -797,7 +813,7 @@
         <v>15</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>37</v>
@@ -806,13 +822,14 @@
         <v>19</v>
       </c>
       <c r="L3"/>
-    </row>
-    <row r="4" spans="1:13" ht="45">
+      <c r="M3" s="11"/>
+    </row>
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>16</v>
@@ -829,7 +846,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -838,13 +855,14 @@
       <c r="L4" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="60">
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>16</v>
@@ -861,17 +879,18 @@
         <v>15</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>37</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L5"/>
-    </row>
-    <row r="6" spans="1:13" ht="60">
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
@@ -893,19 +912,20 @@
         <v>21</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>37</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="31.5">
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -937,7 +957,7 @@
       </c>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:13" ht="135">
+    <row r="8" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -959,7 +979,7 @@
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>40</v>
@@ -969,7 +989,7 @@
       </c>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:13" ht="45">
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -991,19 +1011,19 @@
         <v>27</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>37</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L9" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="31.5">
+    <row r="10" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1025,7 +1045,7 @@
         <v>27</v>
       </c>
       <c r="I10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J10" t="s">
         <v>43</v>
@@ -1035,7 +1055,7 @@
       </c>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="31.5">
+    <row r="11" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1057,7 +1077,7 @@
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>37</v>
@@ -1067,7 +1087,7 @@
       </c>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:13" ht="45">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1097,9 +1117,9 @@
       </c>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:13" ht="47.25">
+    <row r="13" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>60</v>
@@ -1119,22 +1139,22 @@
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>37</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:13" ht="31.5">
+    <row r="14" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>16</v>
@@ -1159,12 +1179,12 @@
       </c>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:13" ht="31.5">
+    <row r="15" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>16</v>
@@ -1178,7 +1198,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I15"/>
       <c r="J15" t="s">
@@ -1189,7 +1209,7 @@
       </c>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:13" ht="31.5">
+    <row r="16" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1211,7 +1231,7 @@
         <v>33</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>37</v>
@@ -1221,7 +1241,7 @@
       </c>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="31.5">
+    <row r="17" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1241,7 +1261,7 @@
         <v>33</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J17" t="s">
         <v>46</v>
@@ -1251,9 +1271,9 @@
       </c>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="31.5">
+    <row r="18" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>32</v>
@@ -1273,10 +1293,10 @@
         <v>33</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Fixed failed script in steam module
</commit_message>
<xml_diff>
--- a/src/test/test-data/STeAMTestData.xlsx
+++ b/src/test/test-data/STeAMTestData.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UC196992\Git\1p-api-automation\src\test\test-data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
@@ -276,14 +271,14 @@
     <t>userID=(OPQA-2407_user.userID)</t>
   </si>
   <si>
-    <t xml:space="preserve">status=200||rc=90063||fn[1].error=Login Failed.  9 more chances are remaining, after that your account will be locked. </t>
+    <t>status=200||rc=90063||fn[1].error={"ErrorCode":"90063","ErrorMessage":"Login Failed.  9 more chances are remaining, after that your account will be locked. "}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,7 +445,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -482,10 +477,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -517,7 +511,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -693,14 +686,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
@@ -717,7 +710,7 @@
     <col min="13" max="13" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -758,7 +751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="60">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
@@ -791,7 +784,7 @@
       </c>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="60">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -824,7 +817,7 @@
       <c r="L3"/>
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="45">
       <c r="A4" s="6" t="s">
         <v>83</v>
       </c>
@@ -857,7 +850,7 @@
       </c>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="60">
       <c r="A5" s="6" t="s">
         <v>69</v>
       </c>
@@ -890,7 +883,7 @@
       <c r="L5"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="60">
       <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
@@ -925,7 +918,7 @@
       </c>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="31.5">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -957,7 +950,7 @@
       </c>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="135">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -989,7 +982,7 @@
       </c>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="45">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1023,7 +1016,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="31.5">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1055,7 +1048,7 @@
       </c>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="31.5">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1087,7 +1080,7 @@
       </c>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="45">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1117,7 +1110,7 @@
       </c>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="47.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1149,7 +1142,7 @@
       </c>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="31.5">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1179,7 +1172,7 @@
       </c>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="31.5">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1209,7 +1202,7 @@
       </c>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="31.5">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1241,7 +1234,7 @@
       </c>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="31.5">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1271,7 +1264,7 @@
       </c>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="31.5">
       <c r="A18" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Modified url for steam testcaes
</commit_message>
<xml_diff>
--- a/src/test/test-data/STeAMTestData.xlsx
+++ b/src/test/test-data/STeAMTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bg00483545\git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="87">
   <si>
     <t>STATUS</t>
   </si>
@@ -226,18 +231,9 @@
     <t>OPQA-1610</t>
   </si>
   <si>
-    <t>USER_NAME=Neon_JDRUser5@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=JDR||USER_LAST_NAME=E5||USER_MIDDLE_NAME=REDDY5||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3235123</t>
-  </si>
-  <si>
-    <t>USER_NAME=Project_NeonUser1@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=Project||USER_LAST_NAME=Neon1||USER_MIDDLE_NAME=TR||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3235123</t>
-  </si>
-  <si>
     <t>Verify that new STeAM user account can be created without first name, last name using STeAM API</t>
   </si>
   <si>
-    <t>USER_NAME=Neon_JDRUser6@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3235124</t>
-  </si>
-  <si>
     <t>OPQA-1418_1</t>
   </si>
   <si>
@@ -272,13 +268,25 @@
   </si>
   <si>
     <t>status=200||rc=90063||fn[1].error={"ErrorCode":"90063","ErrorMessage":"Login Failed.  9 more chances are remaining, after that your account will be locked. "}</t>
+  </si>
+  <si>
+    <t>USER_NAME=Project_NeonUser1@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=Project||USER_LAST_NAME=Neon1||USER_MIDDLE_NAME=TR||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3232233</t>
+  </si>
+  <si>
+    <t>USER_NAME=Project_NeonUser1@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=Project||USER_LAST_NAME=Neon1||USER_MIDDLE_NAME=TR||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3230987</t>
+  </si>
+  <si>
+    <t>USER_NAME=Neon_JDRUser5@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=JDR||USER_LAST_NAME=E5||USER_MIDDLE_NAME=REDDY5||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3232233</t>
+  </si>
+  <si>
+    <t>USER_NAME=Neon_JDRUser6@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3235566</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,7 +453,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,9 +485,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -511,6 +520,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -686,14 +696,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
@@ -710,7 +720,7 @@
     <col min="13" max="13" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -751,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60">
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
@@ -773,7 +783,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
@@ -784,7 +794,7 @@
       </c>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:13" ht="60">
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -806,7 +816,7 @@
         <v>15</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>37</v>
@@ -817,12 +827,12 @@
       <c r="L3"/>
       <c r="M3" s="11"/>
     </row>
-    <row r="4" spans="1:13" ht="45">
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>16</v>
@@ -839,7 +849,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -850,7 +860,7 @@
       </c>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:13" ht="60">
+    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>69</v>
       </c>
@@ -872,7 +882,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>37</v>
@@ -883,7 +893,7 @@
       <c r="L5"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" ht="60">
+    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>40</v>
       </c>
@@ -905,20 +915,20 @@
         <v>21</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>37</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>34</v>
       </c>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="31.5">
+    <row r="7" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -950,7 +960,7 @@
       </c>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:13" ht="135">
+    <row r="8" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -972,7 +982,7 @@
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>40</v>
@@ -982,7 +992,7 @@
       </c>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:13" ht="45">
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1004,19 +1014,19 @@
         <v>27</v>
       </c>
       <c r="I9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>37</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L9" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="31.5">
+    <row r="10" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1038,7 +1048,7 @@
         <v>27</v>
       </c>
       <c r="I10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J10" t="s">
         <v>43</v>
@@ -1048,7 +1058,7 @@
       </c>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="31.5">
+    <row r="11" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1070,7 +1080,7 @@
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>37</v>
@@ -1080,7 +1090,7 @@
       </c>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:13" ht="45">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1110,7 +1120,7 @@
       </c>
       <c r="L12"/>
     </row>
-    <row r="13" spans="1:13" ht="47.25">
+    <row r="13" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1132,17 +1142,17 @@
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>37</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:13" ht="31.5">
+    <row r="14" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1172,7 +1182,7 @@
       </c>
       <c r="L14"/>
     </row>
-    <row r="15" spans="1:13" ht="31.5">
+    <row r="15" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1202,7 +1212,7 @@
       </c>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:13" ht="31.5">
+    <row r="16" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1224,7 +1234,7 @@
         <v>33</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>37</v>
@@ -1234,7 +1244,7 @@
       </c>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" ht="31.5">
+    <row r="17" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1254,7 +1264,7 @@
         <v>33</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J17" t="s">
         <v>46</v>
@@ -1264,9 +1274,9 @@
       </c>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" ht="31.5">
+    <row r="18" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>32</v>
@@ -1286,10 +1296,10 @@
         <v>33</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>20</v>
@@ -1297,11 +1307,7 @@
       <c r="L18"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I4" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
steam test data  file
</commit_message>
<xml_diff>
--- a/src/test/test-data/STeAMTestData.xlsx
+++ b/src/test/test-data/STeAMTestData.xlsx
@@ -270,16 +270,16 @@
     <t>status=200||rc=90063||fn[1].error={"ErrorCode":"90063","ErrorMessage":"Login Failed.  9 more chances are remaining, after that your account will be locked. "}</t>
   </si>
   <si>
-    <t>USER_NAME=Project_NeonUser1@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=Project||USER_LAST_NAME=Neon1||USER_MIDDLE_NAME=TR||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3232233</t>
-  </si>
-  <si>
-    <t>USER_NAME=Project_NeonUser1@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=Project||USER_LAST_NAME=Neon1||USER_MIDDLE_NAME=TR||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3230987</t>
-  </si>
-  <si>
-    <t>USER_NAME=Neon_JDRUser5@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=JDR||USER_LAST_NAME=E5||USER_MIDDLE_NAME=REDDY5||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3232233</t>
-  </si>
-  <si>
-    <t>USER_NAME=Neon_JDRUser6@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_TRUID=655694d8-f72a-4be4-906c-1e53d3235566</t>
+    <t>USER_NAME=Project_NeonUser1@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=Project||USER_LAST_NAME=Neon1||USER_MIDDLE_NAME=TR||USER_TRUID=944694d8-f72a-4be4-906c-1e53d3232098</t>
+  </si>
+  <si>
+    <t>USER_NAME=Project_NeonUser1@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=Project||USER_LAST_NAME=Neon1||USER_MIDDLE_NAME=TR||USER_TRUID=444694d8-f72a-4be4-906c-1e53d3232098</t>
+  </si>
+  <si>
+    <t>USER_NAME=Neon_JDRUser6@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_TRUID=555694d8-f72a-4be4-906c-1e53d3235466</t>
+  </si>
+  <si>
+    <t>USER_NAME=Neon_JDRUser5@1p.com||USER_PASSWORD=1234qwer$$!||PASSWORD_GENERATE=NO||EMAIL_GENERATE=YES||USER_FIRST_NAME=JDR||USER_LAST_NAME=E5||USER_MIDDLE_NAME=REDDY5||USER_TRUID=555694d8-f72a-4be4-906c-1e53d3235466</t>
   </si>
 </sst>
 </file>
@@ -700,7 +700,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +849,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -882,7 +882,7 @@
         <v>15</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>37</v>

</xml_diff>